<commit_message>
Update DN et JE
DN de marde de gestion de mon cul et JE a modifier qui me font chier >:(
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 4/Documentation/Analyse/P04-JE.xlsx
+++ b/Sprint 1/Package 4/Documentation/Analyse/P04-JE.xlsx
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>NoType</t>
-  </si>
-  <si>
-    <t>DescType</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>En cours</t>
   </si>
@@ -39,19 +33,118 @@
     <t>Terminer</t>
   </si>
   <si>
-    <t>Pas encore commencer</t>
-  </si>
-  <si>
     <t>Suspendu</t>
   </si>
   <si>
-    <t>NoTypeTest</t>
-  </si>
-  <si>
-    <t>DescCourteTest</t>
-  </si>
-  <si>
-    <t>DescriptionTest</t>
+    <t>A faire</t>
+  </si>
+  <si>
+    <t>CommentaireStatut</t>
+  </si>
+  <si>
+    <t>NoStatut</t>
+  </si>
+  <si>
+    <t>DescStatut</t>
+  </si>
+  <si>
+    <t>Au cas où une urgence survient et que l'équipe ne peu plus continuer de travailler sur un test en cours</t>
+  </si>
+  <si>
+    <t>CodeTypeTest</t>
+  </si>
+  <si>
+    <t>NomTypeTest</t>
+  </si>
+  <si>
+    <t>DescTypeTest</t>
+  </si>
+  <si>
+    <t>CommentaireTest</t>
+  </si>
+  <si>
+    <t>AnAct</t>
+  </si>
+  <si>
+    <t>Analyse de l'activité</t>
+  </si>
+  <si>
+    <t>ObjectifTypeTest</t>
+  </si>
+  <si>
+    <t>Saisir la réalité et la complexité des activités humaines dans une situation précise</t>
+  </si>
+  <si>
+    <t>Analyse de la demande, Entretiens, Observations ouverte, Observation systématique</t>
+  </si>
+  <si>
+    <t>AuCon</t>
+  </si>
+  <si>
+    <t>Auto confrontation</t>
+  </si>
+  <si>
+    <t>Comprendre comment le joueur contruit mentalement son activité et quels facteurs influencent cette construction</t>
+  </si>
+  <si>
+    <t>Filmer le joueur pendant l'activité et le laisser commenter son comportement en visionnant le film</t>
+  </si>
+  <si>
+    <t>RePhy</t>
+  </si>
+  <si>
+    <t>Recueil des mesures physiologiques</t>
+  </si>
+  <si>
+    <t>Indiquer l'état de vigilance ou émotionnel d'une personne face à une certaine situation</t>
+  </si>
+  <si>
+    <t>Recueillir la fréquence cardiaque, l'activité électrodermal et d'autres mesures d'un joueur en réponse à une certaine situation</t>
+  </si>
+  <si>
+    <t>AnHeu</t>
+  </si>
+  <si>
+    <t>Analyse heuristique</t>
+  </si>
+  <si>
+    <t>Test le respect des règles de l'art et les critères ergonomiques d'un interface</t>
+  </si>
+  <si>
+    <t>Inspecter une interface à partir d'une grille d''heuristiques afin de détecter les aspects positifs et négatifs, réaliser par plusieur ergonomes</t>
+  </si>
+  <si>
+    <t>CoWal</t>
+  </si>
+  <si>
+    <t>Cognitive walkthrough</t>
+  </si>
+  <si>
+    <t>tester la logique interactive du système, évaluer les interfaces d'un jeu</t>
+  </si>
+  <si>
+    <t>Phase de préparation, de d''évaluation et d''analyse</t>
+  </si>
+  <si>
+    <t>EnTre</t>
+  </si>
+  <si>
+    <t>Entretien</t>
+  </si>
+  <si>
+    <t>Déterminer les avis, les jugements, les opinions, les croyances, les émotions par rapport à un sujet précis</t>
+  </si>
+  <si>
+    <t>Prendre un RDV avec un joueur ciblé, interviewer le joueur sur le jeu pour avoir ces avis sur un jeu, analyser ces réaction et réponse</t>
+  </si>
+  <si>
+    <t>test très long à faire à grande échelle</t>
+  </si>
+  <si>
+    <t>FoGro</t>
+  </si>
+  <si>
+    <t>Focus group</t>
   </si>
 </sst>
 </file>
@@ -400,56 +493,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="82.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -459,127 +560,131 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="138.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" customWidth="1"/>
+    <col min="3" max="3" width="94.21875" customWidth="1"/>
+    <col min="4" max="4" width="112.88671875" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="D3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>